<commit_message>
Database Design - 19.10.2024
</commit_message>
<xml_diff>
--- a/java22 database design/Java22 QPhan Database Design.xlsx
+++ b/java22 database design/Java22 QPhan Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java22\3. Database\java22 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88321B5E-1FF4-4A05-8F6A-D07E478E168F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB50752D-D650-4E73-9065-A97D1241B369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="878" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="694" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -254,6 +254,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Quyen Ngoc Phan</author>
     <author>tc={598B10B6-E6F1-40B5-B6AD-C3AD129CB648}</author>
     <author>tc={85B16A7D-4DA7-409D-A477-42471121604E}</author>
     <author>tc={FEB531F8-3F37-41C2-9572-96E04C8ECAC8}</author>
@@ -261,7 +262,32 @@
     <author>tc={15149510-1AD6-4534-986F-C2ED6ADDDE50}</author>
   </authors>
   <commentList>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{598B10B6-E6F1-40B5-B6AD-C3AD129CB648}">
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{2F737CB0-E0CB-4891-AC38-F48F369004EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+C09_PAYMENT_ID
+C09_PAYMENT_NAME</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="1" shapeId="0" xr:uid="{598B10B6-E6F1-40B5-B6AD-C3AD129CB648}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -271,7 +297,7 @@
 Thanh toán online - thẻ ghi nợ</t>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{85B16A7D-4DA7-409D-A477-42471121604E}">
+    <comment ref="M6" authorId="2" shapeId="0" xr:uid="{85B16A7D-4DA7-409D-A477-42471121604E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -286,7 +312,58 @@
 </t>
       </text>
     </comment>
-    <comment ref="C10" authorId="2" shapeId="0" xr:uid="{FEB531F8-3F37-41C2-9572-96E04C8ECAC8}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{5CDBD3A2-85AC-40A6-B006-3617BB8DA63B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mã số thuế
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{F5056F4D-851D-4278-84E4-43EF14C081FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hmm ?
+Không nên UNIQUE
+1 ngày có thể 1 mặt hàng được nhập 2 lần</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="3" shapeId="0" xr:uid="{FEB531F8-3F37-41C2-9572-96E04C8ECAC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -295,7 +372,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="G11" authorId="3" shapeId="0" xr:uid="{9DB5297B-73D2-42AE-9A76-79B839CE1D77}">
+    <comment ref="G11" authorId="4" shapeId="0" xr:uid="{9DB5297B-73D2-42AE-9A76-79B839CE1D77}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -303,7 +380,7 @@
     Lưu lịch sử mua hàng của từng khách hàng</t>
       </text>
     </comment>
-    <comment ref="M18" authorId="4" shapeId="0" xr:uid="{15149510-1AD6-4534-986F-C2ED6ADDDE50}">
+    <comment ref="M18" authorId="5" shapeId="0" xr:uid="{15149510-1AD6-4534-986F-C2ED6ADDDE50}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -550,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="552">
   <si>
     <t>NhanVien</t>
   </si>
@@ -2073,9 +2150,6 @@
   </si>
   <si>
     <t>[100, 120, 140, 160, 180, 200]</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>C12_SIZE_DESC</t>
@@ -2211,12 +2285,24 @@
   <si>
     <t>C13_EMPLOYEE_PASSWORD</t>
   </si>
+  <si>
+    <t>Sau khi thiết kế xong cơ sở dữ liệu vật lý (giấy, bản vẽ, thiết kế) có 2 cách sau đây để tạo ra CSDL vật lý dùng cho coding</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>C09_PAYMENT_METHOD_ID</t>
+  </si>
+  <si>
+    <t>C09_PAYMENT_METHOD_TYPE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2406,6 +2492,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -2675,11 +2768,23 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2693,6 +2798,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2701,24 +2812,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3187,7 +3280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3885,7 +3978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
   <dimension ref="B1:N250"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B56" sqref="B56:I67"/>
     </sheetView>
   </sheetViews>
@@ -5464,16 +5557,16 @@
     </row>
     <row r="72" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="66" t="s">
+      <c r="C73" s="72" t="s">
         <v>277</v>
       </c>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
+      <c r="D73" s="72"/>
+      <c r="E73" s="72"/>
     </row>
     <row r="74" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="66"/>
-      <c r="D74" s="66"/>
-      <c r="E74" s="66"/>
+      <c r="C74" s="72"/>
+      <c r="D74" s="72"/>
+      <c r="E74" s="72"/>
     </row>
     <row r="75" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5497,14 +5590,14 @@
     </row>
     <row r="78" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="66" t="s">
+      <c r="C79" s="72" t="s">
         <v>277</v>
       </c>
-      <c r="D79" s="66"/>
+      <c r="D79" s="72"/>
     </row>
     <row r="80" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="66"/>
-      <c r="D80" s="66"/>
+      <c r="C80" s="72"/>
+      <c r="D80" s="72"/>
     </row>
     <row r="81" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5539,30 +5632,30 @@
       </c>
     </row>
     <row r="86" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="67" t="s">
+      <c r="C86" s="73" t="s">
         <v>283</v>
       </c>
-      <c r="D86" s="66"/>
-      <c r="E86" s="66"/>
-      <c r="F86" s="66"/>
+      <c r="D86" s="72"/>
+      <c r="E86" s="72"/>
+      <c r="F86" s="72"/>
     </row>
     <row r="87" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="66"/>
-      <c r="D87" s="66"/>
-      <c r="E87" s="66"/>
-      <c r="F87" s="66"/>
+      <c r="C87" s="72"/>
+      <c r="D87" s="72"/>
+      <c r="E87" s="72"/>
+      <c r="F87" s="72"/>
     </row>
     <row r="88" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="66"/>
-      <c r="D88" s="66"/>
-      <c r="E88" s="66"/>
-      <c r="F88" s="66"/>
+      <c r="C88" s="72"/>
+      <c r="D88" s="72"/>
+      <c r="E88" s="72"/>
+      <c r="F88" s="72"/>
     </row>
     <row r="89" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="66"/>
-      <c r="D89" s="66"/>
-      <c r="E89" s="66"/>
-      <c r="F89" s="66"/>
+      <c r="C89" s="72"/>
+      <c r="D89" s="72"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="72"/>
     </row>
     <row r="90" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5579,18 +5672,18 @@
       </c>
     </row>
     <row r="93" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="68" t="s">
+      <c r="B93" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="C93" s="68"/>
+      <c r="C93" s="74"/>
     </row>
     <row r="94" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="66"/>
-      <c r="C94" s="66"/>
+      <c r="B94" s="72"/>
+      <c r="C94" s="72"/>
     </row>
     <row r="95" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="66"/>
-      <c r="C95" s="66"/>
+      <c r="B95" s="72"/>
+      <c r="C95" s="72"/>
     </row>
     <row r="96" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5613,11 +5706,11 @@
       </c>
     </row>
     <row r="99" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="69" t="s">
+      <c r="B99" s="71" t="s">
         <v>281</v>
       </c>
-      <c r="C99" s="69"/>
-      <c r="D99" s="69"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="71"/>
       <c r="F99" s="14" t="s">
         <v>112</v>
       </c>
@@ -5632,14 +5725,14 @@
       </c>
     </row>
     <row r="100" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
+      <c r="B100" s="71"/>
+      <c r="C100" s="71"/>
+      <c r="D100" s="71"/>
     </row>
     <row r="101" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="69"/>
-      <c r="C101" s="69"/>
-      <c r="D101" s="69"/>
+      <c r="B101" s="71"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="71"/>
       <c r="F101" s="31" t="s">
         <v>297</v>
       </c>
@@ -5647,7 +5740,7 @@
         <v>253</v>
       </c>
       <c r="I101" s="27" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="102" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6180,7 +6273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02AFA64-4F84-47ED-AB68-8CF3C6F7C8A6}">
   <dimension ref="B1:N80"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -6725,7 +6818,7 @@
       <c r="N28" s="17"/>
     </row>
     <row r="29" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="61"/>
+      <c r="H29" s="60"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
@@ -6982,14 +7075,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
   <dimension ref="B1:P60"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showFormulas="1" topLeftCell="B32" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
@@ -7338,15 +7431,15 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
     </row>
     <row r="18" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -7358,12 +7451,12 @@
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
     </row>
@@ -7375,12 +7468,12 @@
       <c r="K20" s="17"/>
     </row>
     <row r="21" spans="2:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
     </row>
@@ -7395,32 +7488,32 @@
       <c r="K22" s="20"/>
     </row>
     <row r="23" spans="2:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="2:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="2:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="4"/>
@@ -7445,7 +7538,7 @@
     </row>
     <row r="29" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>548</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -7613,8 +7706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1DF7D6-F95C-4B2D-93D8-507FCBA4401D}">
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O8"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7626,7 +7719,7 @@
     <col min="7" max="9" width="28.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="33.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="28.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="36.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="28.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="27" style="1" customWidth="1"/>
@@ -7659,30 +7752,46 @@
     </row>
     <row r="3" spans="2:21" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>505</v>
+        <v>549</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>505</v>
+        <v>549</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>505</v>
+        <v>549</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+        <v>549</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>549</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>549</v>
+      </c>
       <c r="O3" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="P3" s="6"/>
+        <v>549</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>549</v>
+      </c>
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="2:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -7760,7 +7869,7 @@
         <v>443</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J5" s="38" t="s">
         <v>462</v>
@@ -7769,7 +7878,7 @@
         <v>448</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>439</v>
+        <v>550</v>
       </c>
       <c r="M5" s="38" t="s">
         <v>455</v>
@@ -7811,7 +7920,7 @@
       <c r="H6" s="35" t="s">
         <v>444</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="59" t="s">
         <v>458</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -7821,7 +7930,7 @@
         <v>449</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>440</v>
+        <v>551</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>456</v>
@@ -7861,7 +7970,7 @@
       <c r="H7" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="59" t="s">
         <v>459</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -7879,7 +7988,9 @@
       <c r="P7" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="65" t="s">
+        <v>544</v>
+      </c>
       <c r="R7" s="18"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -7897,7 +8008,8 @@
       <c r="G8" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="26" t="s">
         <v>460</v>
       </c>
       <c r="J8" s="26" t="s">
@@ -7910,12 +8022,14 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="65" t="s">
+        <v>546</v>
+      </c>
       <c r="R8" s="18"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -7932,11 +8046,11 @@
         <v>424</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>527</v>
-      </c>
-      <c r="H9" s="60"/>
+        <v>526</v>
+      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
@@ -7949,7 +8063,9 @@
       <c r="P9" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="65" t="s">
+        <v>545</v>
+      </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -7968,6 +8084,7 @@
       <c r="G10" s="3" t="s">
         <v>441</v>
       </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
@@ -7980,7 +8097,9 @@
       <c r="P10" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="Q10" s="18"/>
+      <c r="Q10" s="65" t="s">
+        <v>547</v>
+      </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -8043,7 +8162,6 @@
       <c r="G13" s="26"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -8097,18 +8215,18 @@
       </c>
     </row>
     <row r="17" spans="4:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
       <c r="O17" s="1">
         <v>1</v>
       </c>
@@ -8140,15 +8258,15 @@
       </c>
     </row>
     <row r="19" spans="4:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17">
         <v>3</v>
@@ -8176,15 +8294,15 @@
       </c>
     </row>
     <row r="21" spans="4:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
       <c r="N21" s="17"/>
       <c r="O21" s="1">
         <v>5</v>
@@ -8218,15 +8336,15 @@
       </c>
     </row>
     <row r="23" spans="4:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
       <c r="N23" s="7"/>
       <c r="O23" s="17">
         <v>7</v>
@@ -8239,15 +8357,15 @@
       </c>
     </row>
     <row r="24" spans="4:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
       <c r="N24" s="7"/>
       <c r="O24" s="17">
         <v>8</v>
@@ -8260,15 +8378,15 @@
       </c>
     </row>
     <row r="25" spans="4:18" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
       <c r="K25" s="15"/>
       <c r="L25" s="4"/>
       <c r="P25" s="15"/>
@@ -8467,10 +8585,9 @@
     <row r="59" spans="4:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="4:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="D25:J25"/>
     <mergeCell ref="D17:J17"/>
-    <mergeCell ref="K17:M17"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D21:J21"/>
     <mergeCell ref="D23:J23"/>
@@ -8485,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E20DDFD-7038-45D3-A551-EC11FF1DC63E}">
   <dimension ref="B1:H537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D169" sqref="D169"/>
+    <sheetView topLeftCell="C131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8894,7 +9011,7 @@
         <v>352</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9012,7 +9129,7 @@
         <v>473</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9183,34 +9300,34 @@
     </row>
     <row r="66" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="67" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="70" t="s">
-        <v>509</v>
-      </c>
-      <c r="D67" s="64"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="64"/>
+        <v>508</v>
+      </c>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
     </row>
     <row r="68" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
     </row>
     <row r="69" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
     </row>
     <row r="70" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
-      <c r="E70" s="64"/>
-      <c r="F70" s="64"/>
+      <c r="C70" s="68"/>
+      <c r="D70" s="68"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="68"/>
     </row>
     <row r="71" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9231,7 +9348,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9239,7 +9356,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9247,7 +9364,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="77" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9255,8 +9372,8 @@
       <c r="B78" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C78" s="71" t="s">
-        <v>523</v>
+      <c r="C78" s="61" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9284,7 +9401,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D80" s="29" t="s">
         <v>180</v>
@@ -9304,7 +9421,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D81" s="28" t="s">
         <v>181</v>
@@ -9324,7 +9441,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D82" s="28" t="s">
         <v>182</v>
@@ -9344,7 +9461,7 @@
         <v>4</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D83" s="28" t="s">
         <v>183</v>
@@ -9364,7 +9481,7 @@
         <v>5</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D84" s="28" t="s">
         <v>184</v>
@@ -9384,7 +9501,7 @@
         <v>6</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D85" s="28" t="s">
         <v>185</v>
@@ -9404,7 +9521,7 @@
         <v>7</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D86" s="28" t="s">
         <v>186</v>
@@ -9424,7 +9541,7 @@
         <v>8</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D87" s="28" t="s">
         <v>187</v>
@@ -9444,7 +9561,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D88" s="28" t="s">
         <v>188</v>
@@ -9464,7 +9581,7 @@
         <v>10</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D89" s="28" t="s">
         <v>189</v>
@@ -9499,7 +9616,7 @@
         <v>436</v>
       </c>
       <c r="F92" s="26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>441</v>
@@ -9510,51 +9627,51 @@
     </row>
     <row r="93" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="C93" s="28" t="s">
         <v>524</v>
-      </c>
-      <c r="C93" s="28" t="s">
-        <v>525</v>
       </c>
       <c r="D93" s="28">
         <v>258369741</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F93" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="G93" s="28" t="s">
         <v>528</v>
       </c>
-      <c r="G93" s="28" t="s">
+      <c r="H93" s="28" t="s">
         <v>529</v>
-      </c>
-      <c r="H93" s="28" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="94" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="28"/>
       <c r="C94" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D94" s="28"/>
       <c r="E94" s="28"/>
       <c r="F94" s="28"/>
       <c r="G94" s="28"/>
       <c r="H94" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="95" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="28"/>
       <c r="C95" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D95" s="28"/>
       <c r="E95" s="28"/>
       <c r="F95" s="28"/>
       <c r="G95" s="28"/>
       <c r="H95" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="96" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9575,21 +9692,21 @@
       </c>
     </row>
     <row r="99" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="69" t="s">
+      <c r="B99" s="71" t="s">
         <v>281</v>
       </c>
-      <c r="C99" s="69"/>
-      <c r="D99" s="69"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="71"/>
     </row>
     <row r="100" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
+      <c r="B100" s="71"/>
+      <c r="C100" s="71"/>
+      <c r="D100" s="71"/>
     </row>
     <row r="101" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="69"/>
-      <c r="C101" s="69"/>
-      <c r="D101" s="69"/>
+      <c r="B101" s="71"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="71"/>
     </row>
     <row r="102" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="28">
@@ -10149,7 +10266,7 @@
     </row>
     <row r="154" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="38" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>458</v>
@@ -10161,14 +10278,14 @@
         <v>460</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="155" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="28" t="s">
         <v>492</v>
       </c>
-      <c r="C155" s="74" t="s">
+      <c r="C155" s="64" t="s">
         <v>297</v>
       </c>
       <c r="D155" s="28"/>
@@ -10176,12 +10293,12 @@
         <v>253</v>
       </c>
       <c r="F155" s="28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="156" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
-      <c r="C156" s="74" t="s">
+      <c r="C156" s="64" t="s">
         <v>298</v>
       </c>
       <c r="D156" s="28"/>
@@ -10194,7 +10311,7 @@
     </row>
     <row r="157" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="28"/>
-      <c r="C157" s="74" t="s">
+      <c r="C157" s="64" t="s">
         <v>299</v>
       </c>
       <c r="D157" s="28"/>
@@ -10207,7 +10324,7 @@
     </row>
     <row r="158" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="28"/>
-      <c r="C158" s="74" t="s">
+      <c r="C158" s="64" t="s">
         <v>282</v>
       </c>
       <c r="D158" s="28"/>
@@ -10220,7 +10337,7 @@
     </row>
     <row r="159" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="28"/>
-      <c r="C159" s="74" t="s">
+      <c r="C159" s="64" t="s">
         <v>301</v>
       </c>
       <c r="D159" s="28"/>
@@ -10231,7 +10348,7 @@
     </row>
     <row r="160" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="73" t="s">
+      <c r="B161" s="63" t="s">
         <v>461</v>
       </c>
     </row>
@@ -10251,14 +10368,14 @@
     </row>
     <row r="163" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="164" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C164" s="69" t="s">
-        <v>542</v>
-      </c>
-      <c r="D164" s="69"/>
+      <c r="C164" s="71" t="s">
+        <v>541</v>
+      </c>
+      <c r="D164" s="71"/>
     </row>
     <row r="165" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="73" t="s">
+      <c r="B166" s="63" t="s">
         <v>454</v>
       </c>
       <c r="E166" s="2" t="s">
@@ -10267,10 +10384,10 @@
     </row>
     <row r="167" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="38" t="s">
+        <v>542</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>544</v>
       </c>
       <c r="E167" s="38" t="s">
         <v>467</v>
@@ -10361,7 +10478,7 @@
     </row>
     <row r="175" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="73" t="s">
+      <c r="B176" s="63" t="s">
         <v>474</v>
       </c>
     </row>
@@ -10373,16 +10490,16 @@
         <v>476</v>
       </c>
       <c r="D177" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="E177" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="E177" s="3" t="s">
+      <c r="F177" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="F177" s="3" t="s">
+      <c r="G177" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="G177" s="3" t="s">
-        <v>548</v>
       </c>
       <c r="H177" s="4" t="s">
         <v>477</v>
@@ -11579,7 +11696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C31D8E1-EE07-4077-BEA3-A61BD671C8B6}">
   <dimension ref="A3:J37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B22" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B12" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -12080,29 +12197,29 @@
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="39" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F33" s="39"/>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" s="50" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="62" t="s">
         <v>536</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E36" s="72" t="s">
-        <v>537</v>
       </c>
       <c r="H36" s="39"/>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Database - Refresh Test Data - 19.10.2024
</commit_message>
<xml_diff>
--- a/java22 database design/Java22 QPhan Database Design.xlsx
+++ b/java22 database design/Java22 QPhan Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java22\3. Database\java22 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB50752D-D650-4E73-9065-A97D1241B369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58158543-B31B-4FCC-A047-57023123ECEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="694" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="901" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -3978,8 +3978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
   <dimension ref="B1:N250"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:I67"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6149,70 +6149,70 @@
     <row r="142" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="144" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" s="27" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="209" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="210" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="211" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7706,8 +7706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1DF7D6-F95C-4B2D-93D8-507FCBA4401D}">
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8602,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E20DDFD-7038-45D3-A551-EC11FF1DC63E}">
   <dimension ref="B1:H537"/>
   <sheetViews>
-    <sheetView topLeftCell="C131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Database - Refresh Test Data - 20.10.2024
</commit_message>
<xml_diff>
--- a/java22 database design/Java22 QPhan Database Design.xlsx
+++ b/java22 database design/Java22 QPhan Database Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java22\3. Database\java22 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58158543-B31B-4FCC-A047-57023123ECEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE5FF7E-357E-4DDE-84AB-7D058AB496AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="901" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
     Lưu lịch sử mua hàng của từng khách hàng</t>
       </text>
     </comment>
-    <comment ref="C167" authorId="3" shapeId="0" xr:uid="{BE51FF11-58CB-48AB-87EE-2CE40C2B1E43}">
+    <comment ref="C164" authorId="3" shapeId="0" xr:uid="{BE51FF11-58CB-48AB-87EE-2CE40C2B1E43}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -438,7 +438,7 @@
     Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</t>
       </text>
     </comment>
-    <comment ref="B176" authorId="4" shapeId="0" xr:uid="{1889A6B9-A887-4E66-B154-B6836B46BB11}">
+    <comment ref="B173" authorId="4" shapeId="0" xr:uid="{1889A6B9-A887-4E66-B154-B6836B46BB11}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -446,7 +446,7 @@
     Không cần thuộc phòng ban, làm được mọi chức năng</t>
       </text>
     </comment>
-    <comment ref="H177" authorId="5" shapeId="0" xr:uid="{3E0884F8-12AF-4883-9EE3-1199104BAB36}">
+    <comment ref="H174" authorId="5" shapeId="0" xr:uid="{3E0884F8-12AF-4883-9EE3-1199104BAB36}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -627,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="553">
   <si>
     <t>NhanVien</t>
   </si>
@@ -2117,9 +2117,6 @@
   </si>
   <si>
     <t>Mặt Hàng 1-4</t>
-  </si>
-  <si>
-    <t>Mặt Hàng 1-8</t>
   </si>
   <si>
     <t>Mặt Hàng 9-12</t>
@@ -2296,6 +2293,12 @@
   </si>
   <si>
     <t>C09_PAYMENT_METHOD_TYPE</t>
+  </si>
+  <si>
+    <t>Mặt Hàng 5-8</t>
+  </si>
+  <si>
+    <t>[red, yelllow, blue, green, orange]</t>
   </si>
 </sst>
 </file>
@@ -3231,13 +3234,13 @@
   <threadedComment ref="H92" dT="2024-09-22T10:28:34.25" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{7E594673-E98C-4AE5-A575-6252DC5C62D3}">
     <text>Lưu lịch sử mua hàng của từng khách hàng</text>
   </threadedComment>
-  <threadedComment ref="C167" dT="2024-04-06T14:25:21.49" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{BE51FF11-58CB-48AB-87EE-2CE40C2B1E43}">
+  <threadedComment ref="C164" dT="2024-04-06T14:25:21.49" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{BE51FF11-58CB-48AB-87EE-2CE40C2B1E43}">
     <text>Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</text>
   </threadedComment>
-  <threadedComment ref="B176" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1889A6B9-A887-4E66-B154-B6836B46BB11}">
+  <threadedComment ref="B173" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1889A6B9-A887-4E66-B154-B6836B46BB11}">
     <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
   </threadedComment>
-  <threadedComment ref="H177" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3E0884F8-12AF-4883-9EE3-1199104BAB36}">
+  <threadedComment ref="H174" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3E0884F8-12AF-4883-9EE3-1199104BAB36}">
     <text>NhanVien, Quan Ly</text>
   </threadedComment>
 </ThreadedComments>
@@ -5740,7 +5743,7 @@
         <v>253</v>
       </c>
       <c r="I101" s="27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="102" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7538,7 +7541,7 @@
     </row>
     <row r="29" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -7707,7 +7710,7 @@
   <dimension ref="B1:U60"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B3" sqref="B3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7752,45 +7755,45 @@
     </row>
     <row r="3" spans="2:21" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Q3" s="6"/>
     </row>
@@ -7869,7 +7872,7 @@
         <v>443</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J5" s="38" t="s">
         <v>462</v>
@@ -7878,7 +7881,7 @@
         <v>448</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="M5" s="38" t="s">
         <v>455</v>
@@ -7930,7 +7933,7 @@
         <v>449</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>456</v>
@@ -7989,7 +7992,7 @@
         <v>478</v>
       </c>
       <c r="Q7" s="65" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="R7" s="18"/>
       <c r="S7" s="3"/>
@@ -8022,13 +8025,13 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>478</v>
       </c>
       <c r="Q8" s="65" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="R8" s="18"/>
       <c r="S8" s="3"/>
@@ -8046,11 +8049,11 @@
         <v>424</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
@@ -8064,7 +8067,7 @@
         <v>478</v>
       </c>
       <c r="Q9" s="65" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -8098,7 +8101,7 @@
         <v>478</v>
       </c>
       <c r="Q10" s="65" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -8600,10 +8603,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E20DDFD-7038-45D3-A551-EC11FF1DC63E}">
-  <dimension ref="B1:H537"/>
+  <dimension ref="B1:H534"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView tabSelected="1" topLeftCell="E62" zoomScale="191" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8612,7 +8615,7 @@
     <col min="2" max="2" width="28.7109375" style="27" customWidth="1"/>
     <col min="3" max="3" width="29" style="27" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="27" customWidth="1"/>
     <col min="6" max="6" width="43" style="27" customWidth="1"/>
     <col min="7" max="7" width="30.85546875" style="27" customWidth="1"/>
     <col min="8" max="8" width="30.5703125" style="27" customWidth="1"/>
@@ -9011,7 +9014,7 @@
         <v>352</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9045,65 +9048,65 @@
         <v>1</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="28"/>
       <c r="C46" s="28" t="s">
-        <v>494</v>
+        <v>551</v>
       </c>
       <c r="D46" s="28">
         <v>2</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="28"/>
       <c r="C47" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D47" s="28">
         <v>3</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G47" s="28"/>
     </row>
     <row r="48" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="28"/>
       <c r="C48" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D48" s="28">
         <v>4</v>
       </c>
       <c r="E48" s="28"/>
       <c r="F48" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G48" s="28"/>
     </row>
     <row r="49" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="28"/>
       <c r="C49" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D49" s="28">
         <v>5</v>
@@ -9129,7 +9132,7 @@
         <v>473</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9277,6 +9280,9 @@
       <c r="B64" s="2" t="s">
         <v>419</v>
       </c>
+      <c r="E64" s="27" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="65" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="38" t="s">
@@ -9300,12 +9306,12 @@
     </row>
     <row r="66" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="67" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="70" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D67" s="68"/>
       <c r="E67" s="68"/>
@@ -9348,7 +9354,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9356,7 +9362,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9364,7 +9370,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="77" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9373,7 +9379,7 @@
         <v>447</v>
       </c>
       <c r="C78" s="61" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9401,7 +9407,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D80" s="29" t="s">
         <v>180</v>
@@ -9421,7 +9427,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D81" s="28" t="s">
         <v>181</v>
@@ -9441,7 +9447,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D82" s="28" t="s">
         <v>182</v>
@@ -9461,7 +9467,7 @@
         <v>4</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D83" s="28" t="s">
         <v>183</v>
@@ -9481,7 +9487,7 @@
         <v>5</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D84" s="28" t="s">
         <v>184</v>
@@ -9501,7 +9507,7 @@
         <v>6</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D85" s="28" t="s">
         <v>185</v>
@@ -9521,7 +9527,7 @@
         <v>7</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D86" s="28" t="s">
         <v>186</v>
@@ -9541,7 +9547,7 @@
         <v>8</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D87" s="28" t="s">
         <v>187</v>
@@ -9561,7 +9567,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D88" s="28" t="s">
         <v>188</v>
@@ -9581,7 +9587,7 @@
         <v>10</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D89" s="28" t="s">
         <v>189</v>
@@ -9616,7 +9622,7 @@
         <v>436</v>
       </c>
       <c r="F92" s="26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>441</v>
@@ -9627,51 +9633,51 @@
     </row>
     <row r="93" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="C93" s="28" t="s">
         <v>523</v>
-      </c>
-      <c r="C93" s="28" t="s">
-        <v>524</v>
       </c>
       <c r="D93" s="28">
         <v>258369741</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F93" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="G93" s="28" t="s">
         <v>527</v>
       </c>
-      <c r="G93" s="28" t="s">
+      <c r="H93" s="28" t="s">
         <v>528</v>
-      </c>
-      <c r="H93" s="28" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="94" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="28"/>
       <c r="C94" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D94" s="28"/>
       <c r="E94" s="28"/>
       <c r="F94" s="28"/>
       <c r="G94" s="28"/>
       <c r="H94" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="95" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="28"/>
       <c r="C95" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D95" s="28"/>
       <c r="E95" s="28"/>
       <c r="F95" s="28"/>
       <c r="G95" s="28"/>
       <c r="H95" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="96" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9692,28 +9698,44 @@
       </c>
     </row>
     <row r="99" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="71" t="s">
-        <v>281</v>
-      </c>
-      <c r="C99" s="71"/>
-      <c r="D99" s="71"/>
+      <c r="B99" s="28">
+        <v>1</v>
+      </c>
+      <c r="C99" s="28">
+        <v>1</v>
+      </c>
+      <c r="D99" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="100" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="71"/>
-      <c r="C100" s="71"/>
-      <c r="D100" s="71"/>
+      <c r="B100" s="28">
+        <v>1</v>
+      </c>
+      <c r="C100" s="28">
+        <v>3</v>
+      </c>
+      <c r="D100" s="28">
+        <v>4</v>
+      </c>
     </row>
     <row r="101" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="71"/>
-      <c r="C101" s="71"/>
-      <c r="D101" s="71"/>
+      <c r="B101" s="28">
+        <v>2</v>
+      </c>
+      <c r="C101" s="28">
+        <v>4</v>
+      </c>
+      <c r="D101" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="102" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C102" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D102" s="28">
         <v>2</v>
@@ -9721,10 +9743,10 @@
     </row>
     <row r="103" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C103" s="28">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D103" s="28">
         <v>4</v>
@@ -9732,21 +9754,21 @@
     </row>
     <row r="104" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C104" s="28">
+        <v>2</v>
+      </c>
+      <c r="D104" s="28">
         <v>4</v>
-      </c>
-      <c r="D104" s="28">
-        <v>2</v>
       </c>
     </row>
     <row r="105" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C105" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D105" s="28">
         <v>2</v>
@@ -9754,10 +9776,10 @@
     </row>
     <row r="106" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C106" s="28">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D106" s="28">
         <v>4</v>
@@ -9765,35 +9787,35 @@
     </row>
     <row r="107" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C107" s="28">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="D107" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C108" s="28">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D108" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C109" s="28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D109" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9801,7 +9823,7 @@
         <v>5</v>
       </c>
       <c r="C110" s="28">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="D110" s="28">
         <v>1</v>
@@ -9809,32 +9831,32 @@
     </row>
     <row r="111" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C111" s="28">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D111" s="28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="28">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C112" s="28">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D112" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C113" s="28">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D113" s="28">
         <v>1</v>
@@ -9842,10 +9864,10 @@
     </row>
     <row r="114" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C114" s="28">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D114" s="28">
         <v>1</v>
@@ -9853,10 +9875,10 @@
     </row>
     <row r="115" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="28">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C115" s="28">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D115" s="28">
         <v>2</v>
@@ -9864,32 +9886,32 @@
     </row>
     <row r="116" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C116" s="28">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="D116" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C117" s="28">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D117" s="28">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C118" s="28">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="D118" s="28">
         <v>2</v>
@@ -9900,10 +9922,10 @@
         <v>9</v>
       </c>
       <c r="C119" s="28">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="D119" s="28">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9911,18 +9933,18 @@
         <v>9</v>
       </c>
       <c r="C120" s="28">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D120" s="28">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C121" s="28">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D121" s="28">
         <v>2</v>
@@ -9930,46 +9952,46 @@
     </row>
     <row r="122" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C122" s="28">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D122" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="28">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C123" s="28">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D123" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C124" s="28">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D124" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C125" s="28">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D125" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9977,7 +9999,7 @@
         <v>11</v>
       </c>
       <c r="C126" s="28">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D126" s="28">
         <v>2</v>
@@ -9988,10 +10010,10 @@
         <v>11</v>
       </c>
       <c r="C127" s="28">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="D127" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9999,117 +10021,117 @@
         <v>11</v>
       </c>
       <c r="C128" s="28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D128" s="28">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="28">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C129" s="28">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D129" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="28">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C130" s="28">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="D130" s="28">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="28">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C131" s="28">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D131" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="28">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C132" s="28">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D132" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C133" s="28">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="D133" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C134" s="28">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D134" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="28">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C135" s="28">
+        <v>9</v>
+      </c>
+      <c r="D135" s="28">
         <v>5</v>
-      </c>
-      <c r="D135" s="28">
-        <v>2</v>
       </c>
     </row>
     <row r="136" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="28">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C136" s="28">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D136" s="28">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="28">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C137" s="28">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D137" s="28">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C138" s="28">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D138" s="28">
         <v>5</v>
@@ -10117,13 +10139,13 @@
     </row>
     <row r="139" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C139" s="28">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="D139" s="28">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10131,392 +10153,428 @@
         <v>16</v>
       </c>
       <c r="C140" s="28">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D140" s="28">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="28">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C141" s="28">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D141" s="28">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="28">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C142" s="28">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D142" s="28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="28">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C143" s="28">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D143" s="28">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="28">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C144" s="28">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D144" s="28">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="28">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C145" s="28">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="D145" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="28">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C146" s="28">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="D146" s="28">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="28">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C147" s="28">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="D147" s="28">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="28">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C148" s="28">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D148" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="28">
-        <v>20</v>
-      </c>
-      <c r="C149" s="28">
-        <v>30</v>
-      </c>
-      <c r="D149" s="28">
-        <v>5</v>
-      </c>
-    </row>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="150" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="28">
-        <v>20</v>
-      </c>
-      <c r="C150" s="28">
-        <v>100</v>
-      </c>
-      <c r="D150" s="28">
-        <v>9</v>
+      <c r="B150" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="151" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="28">
-        <v>20</v>
-      </c>
-      <c r="C151" s="28">
-        <v>70</v>
-      </c>
-      <c r="D151" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B151" s="38" t="s">
+        <v>539</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="C152" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="D152" s="28"/>
+      <c r="E152" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="F152" s="28" t="s">
+        <v>537</v>
+      </c>
+    </row>
     <row r="153" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="2" t="s">
-        <v>457</v>
+      <c r="B153" s="28"/>
+      <c r="C153" s="64" t="s">
+        <v>298</v>
+      </c>
+      <c r="D153" s="28"/>
+      <c r="E153" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="F153" s="29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="38" t="s">
-        <v>540</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>539</v>
+      <c r="B154" s="28"/>
+      <c r="C154" s="64" t="s">
+        <v>299</v>
+      </c>
+      <c r="D154" s="28"/>
+      <c r="E154" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="F154" s="29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="28" t="s">
-        <v>492</v>
-      </c>
+      <c r="B155" s="28"/>
       <c r="C155" s="64" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D155" s="28"/>
       <c r="E155" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="F155" s="28" t="s">
-        <v>538</v>
+        <v>296</v>
+      </c>
+      <c r="F155" s="29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
       <c r="C156" s="64" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D156" s="28"/>
       <c r="E156" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="F156" s="29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="28"/>
-      <c r="C157" s="64" t="s">
-        <v>299</v>
-      </c>
-      <c r="D157" s="28"/>
-      <c r="E157" s="28" t="s">
-        <v>295</v>
-      </c>
-      <c r="F157" s="29" t="s">
-        <v>14</v>
-      </c>
-    </row>
+        <v>300</v>
+      </c>
+      <c r="F156" s="28"/>
+    </row>
+    <row r="157" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="158" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="28"/>
-      <c r="C158" s="64" t="s">
-        <v>282</v>
-      </c>
-      <c r="D158" s="28"/>
-      <c r="E158" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="F158" s="29" t="s">
-        <v>14</v>
+      <c r="B158" s="63" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="159" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="28"/>
-      <c r="C159" s="64" t="s">
-        <v>301</v>
-      </c>
-      <c r="D159" s="28"/>
-      <c r="E159" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="F159" s="28"/>
+      <c r="B159" s="38" t="s">
+        <v>462</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E159" s="26" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="160" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="63" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="162" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="38" t="s">
-        <v>462</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="E162" s="26" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="163" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C164" s="71" t="s">
+    <row r="161" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C161" s="71" t="s">
+        <v>540</v>
+      </c>
+      <c r="D161" s="71"/>
+    </row>
+    <row r="162" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="63" t="s">
+        <v>454</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="38" t="s">
         <v>541</v>
       </c>
-      <c r="D164" s="71"/>
-    </row>
-    <row r="165" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="63" t="s">
-        <v>454</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="167" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="38" t="s">
+      <c r="C164" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="E164" s="38" t="s">
+        <v>467</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="28">
+        <v>1</v>
+      </c>
+      <c r="C165" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="E165" s="28">
+        <v>1</v>
+      </c>
+      <c r="F165" s="28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="28">
+        <v>2</v>
+      </c>
+      <c r="C166" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="E166" s="28">
+        <v>2</v>
+      </c>
+      <c r="F166" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="28">
+        <v>3</v>
+      </c>
+      <c r="C167" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="E167" s="28">
+        <v>3</v>
+      </c>
+      <c r="F167" s="28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="28">
+        <v>4</v>
+      </c>
+      <c r="C168" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E168" s="28">
+        <v>4</v>
+      </c>
+      <c r="F168" s="28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="169" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="28">
+        <v>5</v>
+      </c>
+      <c r="C169" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="28">
+        <v>6</v>
+      </c>
+      <c r="C170" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="28">
+        <v>7</v>
+      </c>
+      <c r="C171" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="172" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="63" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="174" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="38" t="s">
+        <v>475</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D174" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="E167" s="38" t="s">
-        <v>467</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="168" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="28">
-        <v>1</v>
-      </c>
-      <c r="C168" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E168" s="28">
-        <v>1</v>
-      </c>
-      <c r="F168" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="169" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="28">
-        <v>2</v>
-      </c>
-      <c r="C169" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E169" s="28">
-        <v>2</v>
-      </c>
-      <c r="F169" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="170" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="28">
+      <c r="E174" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="H174" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="175" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B175" s="28">
+        <v>1</v>
+      </c>
+      <c r="C175" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D175" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="E175" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="F175" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="G175" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="H175" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="28">
+        <v>2</v>
+      </c>
+      <c r="C176" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="D176" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E176" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="F176" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="G176" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="H176" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="28">
         <v>3</v>
       </c>
-      <c r="C170" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="E170" s="28">
-        <v>3</v>
-      </c>
-      <c r="F170" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="28">
-        <v>4</v>
-      </c>
-      <c r="C171" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="E171" s="28">
-        <v>4</v>
-      </c>
-      <c r="F171" s="28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="172" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="28">
-        <v>5</v>
-      </c>
-      <c r="C172" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="173" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="28">
-        <v>6</v>
-      </c>
-      <c r="C173" s="28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="174" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="28">
-        <v>7</v>
-      </c>
-      <c r="C174" s="28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="63" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="177" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="38" t="s">
-        <v>475</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="F177" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="G177" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="H177" s="4" t="s">
-        <v>477</v>
+      <c r="C177" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="D177" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="E177" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="F177" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="G177" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="H177" s="28">
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C178" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="D178" s="29" t="s">
-        <v>263</v>
+        <v>255</v>
+      </c>
+      <c r="D178" s="28" t="s">
+        <v>285</v>
       </c>
       <c r="E178" s="28" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F178" s="28">
         <v>123456789</v>
@@ -10530,16 +10588,16 @@
     </row>
     <row r="179" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C179" s="28" t="s">
-        <v>254</v>
-      </c>
-      <c r="D179" s="28" t="s">
-        <v>264</v>
+        <v>257</v>
+      </c>
+      <c r="D179" s="29" t="s">
+        <v>291</v>
       </c>
       <c r="E179" s="28" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F179" s="28">
         <v>123456789</v>
@@ -10553,16 +10611,16 @@
     </row>
     <row r="180" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="28">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C180" s="28" t="s">
-        <v>256</v>
-      </c>
-      <c r="D180" s="29" t="s">
-        <v>284</v>
+        <v>258</v>
+      </c>
+      <c r="D180" s="28" t="s">
+        <v>286</v>
       </c>
       <c r="E180" s="28" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F180" s="28">
         <v>123456789</v>
@@ -10571,21 +10629,21 @@
         <v>220</v>
       </c>
       <c r="H180" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="28">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D181" s="28" t="s">
-        <v>285</v>
+        <v>259</v>
+      </c>
+      <c r="D181" s="29" t="s">
+        <v>287</v>
       </c>
       <c r="E181" s="28" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F181" s="28">
         <v>123456789</v>
@@ -10594,21 +10652,21 @@
         <v>220</v>
       </c>
       <c r="H181" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C182" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="D182" s="29" t="s">
-        <v>291</v>
+        <v>260</v>
+      </c>
+      <c r="D182" s="28" t="s">
+        <v>288</v>
       </c>
       <c r="E182" s="28" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F182" s="28">
         <v>123456789</v>
@@ -10617,21 +10675,21 @@
         <v>220</v>
       </c>
       <c r="H182" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="28">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C183" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="D183" s="28" t="s">
-        <v>286</v>
+        <v>261</v>
+      </c>
+      <c r="D183" s="29" t="s">
+        <v>289</v>
       </c>
       <c r="E183" s="28" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F183" s="28">
         <v>123456789</v>
@@ -10645,16 +10703,16 @@
     </row>
     <row r="184" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="28">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C184" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D184" s="29" t="s">
-        <v>287</v>
+        <v>262</v>
+      </c>
+      <c r="D184" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="E184" s="28" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F184" s="28">
         <v>123456789</v>
@@ -10663,78 +10721,12 @@
         <v>220</v>
       </c>
       <c r="H184" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="28">
-        <v>8</v>
-      </c>
-      <c r="C185" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="D185" s="28" t="s">
-        <v>288</v>
-      </c>
-      <c r="E185" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="F185" s="28">
-        <v>123456789</v>
-      </c>
-      <c r="G185" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="H185" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="186" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="28">
-        <v>9</v>
-      </c>
-      <c r="C186" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="D186" s="29" t="s">
-        <v>289</v>
-      </c>
-      <c r="E186" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="F186" s="28">
-        <v>123456789</v>
-      </c>
-      <c r="G186" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="H186" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="28">
-        <v>10</v>
-      </c>
-      <c r="C187" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="D187" s="28" t="s">
-        <v>290</v>
-      </c>
-      <c r="E187" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="F187" s="28">
-        <v>123456789</v>
-      </c>
-      <c r="G187" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="H187" s="28">
         <v>4</v>
       </c>
     </row>
+    <row r="185" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="188" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="189" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="190" spans="2:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11082,14 +11074,10 @@
     <row r="532" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="533" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="534" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="C67:F70"/>
-    <mergeCell ref="B99:D101"/>
-    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C161:D161"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12197,29 +12185,29 @@
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="39" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F33" s="39"/>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36" s="62" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H36" s="39"/>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>